<commit_message>
Refactored. Checked templating is running and generated application works.
</commit_message>
<xml_diff>
--- a/template/AppDefinition.xlsx
+++ b/template/AppDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xltemplating\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538D9B8B-0C95-4564-97EF-4AD7E9799E75}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC854A7F-E332-4B06-AA03-8A1D1ABA39FC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="335">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -1264,6 +1264,10 @@
   </si>
   <si>
     <t>.xtmpl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>basePackage</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1717,10 +1721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B94FD66-5506-4955-9186-3FED46B0C0CF}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1764,6 +1768,14 @@
       </c>
       <c r="D4" t="s">
         <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" t="s">
+        <v>334</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3573,10 +3585,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3666,173 +3678,173 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="W3" s="7"/>
-    </row>
-    <row r="4" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="W4" s="7"/>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E3" s="4" t="str">
+        <f>C3</f>
+        <v>Template</v>
+      </c>
+      <c r="G3" s="3" t="str">
+        <f>LOWER(B3)</f>
+        <v>templatemanagement</v>
+      </c>
+      <c r="H3" s="3" t="str">
+        <f>Application!$D$5&amp;"."&amp;G3</f>
+        <v>com.templengine.templatemanagement</v>
+      </c>
+      <c r="J3" s="3" t="str">
+        <f>H3&amp;".entity"</f>
+        <v>com.templengine.templatemanagement.entity</v>
+      </c>
+      <c r="K3" s="3" t="str">
+        <f>C3</f>
+        <v>Template</v>
+      </c>
+      <c r="M3" s="3" t="str">
+        <f>H3&amp;".dao"</f>
+        <v>com.templengine.templatemanagement.dao</v>
+      </c>
+      <c r="N3" s="3" t="str">
+        <f>C3&amp;"Dao"</f>
+        <v>TemplateDao</v>
+      </c>
+      <c r="P3" s="3" t="str">
+        <f>M3&amp;".mapper"</f>
+        <v>com.templengine.templatemanagement.dao.mapper</v>
+      </c>
+      <c r="Q3" s="3" t="str">
+        <f>K3&amp;"Mapper"</f>
+        <v>TemplateMapper</v>
+      </c>
+      <c r="S3" s="3" t="str">
+        <f>M3&amp;".mapper.gen"</f>
+        <v>com.templengine.templatemanagement.dao.mapper.gen</v>
+      </c>
+      <c r="T3" s="3" t="str">
+        <f>K3&amp;"MapperGen"</f>
+        <v>TemplateMapperGen</v>
+      </c>
+      <c r="V3" t="s">
+        <v>279</v>
+      </c>
+      <c r="W3" s="7" t="str">
+        <f>"/"&amp;LOWER(B3)&amp;V3</f>
+        <v>/templatemanagement/templates</v>
+      </c>
+      <c r="X3" s="3" t="str">
+        <f>H3&amp;".api"</f>
+        <v>com.templengine.templatemanagement.api</v>
+      </c>
+      <c r="Y3" s="3" t="str">
+        <f>C3&amp;"Api"</f>
+        <v>TemplateApi</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E4" s="4" t="str">
+        <f t="shared" ref="E4" si="0">C4</f>
+        <v>TemplateParameter</v>
+      </c>
+      <c r="G4" s="3" t="str">
+        <f t="shared" ref="G4" si="1">LOWER(B4)</f>
+        <v>templatemanagement</v>
+      </c>
+      <c r="H4" s="3" t="str">
+        <f>Application!$D$5&amp;"."&amp;G4</f>
+        <v>com.templengine.templatemanagement</v>
+      </c>
+      <c r="J4" s="3" t="str">
+        <f t="shared" ref="J4" si="2">H4&amp;".entity"</f>
+        <v>com.templengine.templatemanagement.entity</v>
+      </c>
+      <c r="K4" s="3" t="str">
+        <f t="shared" ref="K4" si="3">C4</f>
+        <v>TemplateParameter</v>
+      </c>
+      <c r="M4" s="3" t="str">
+        <f t="shared" ref="M4" si="4">H4&amp;".dao"</f>
+        <v>com.templengine.templatemanagement.dao</v>
+      </c>
+      <c r="N4" s="3" t="str">
+        <f t="shared" ref="N4" si="5">C4&amp;"Dao"</f>
+        <v>TemplateParameterDao</v>
+      </c>
+      <c r="P4" s="3" t="str">
+        <f t="shared" ref="P4" si="6">M4&amp;".mapper"</f>
+        <v>com.templengine.templatemanagement.dao.mapper</v>
+      </c>
+      <c r="Q4" s="3" t="str">
+        <f t="shared" ref="Q4" si="7">K4&amp;"Mapper"</f>
+        <v>TemplateParameterMapper</v>
+      </c>
+      <c r="S4" s="3" t="str">
+        <f t="shared" ref="S4" si="8">M4&amp;".mapper.gen"</f>
+        <v>com.templengine.templatemanagement.dao.mapper.gen</v>
+      </c>
+      <c r="T4" s="3" t="str">
+        <f t="shared" ref="T4" si="9">K4&amp;"MapperGen"</f>
+        <v>TemplateParameterMapperGen</v>
+      </c>
+      <c r="V4" t="s">
+        <v>280</v>
+      </c>
+      <c r="W4" s="7" t="str">
+        <f t="shared" ref="W4" si="10">"/"&amp;LOWER(B4)&amp;V4</f>
+        <v>/templatemanagement/templates/{templateId}/parameters</v>
+      </c>
+      <c r="X4" s="3" t="str">
+        <f t="shared" ref="X4" si="11">H4&amp;".api"</f>
+        <v>com.templengine.templatemanagement.api</v>
+      </c>
+      <c r="Y4" s="3" t="str">
+        <f t="shared" ref="Y4" si="12">C4&amp;"Api"</f>
+        <v>TemplateParameterApi</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C5" t="s">
-        <v>276</v>
-      </c>
-      <c r="E5" s="4" t="str">
-        <f>C5</f>
-        <v>Template</v>
-      </c>
-      <c r="G5" s="3" t="str">
-        <f>LOWER(B5)</f>
-        <v>templatemanagement</v>
-      </c>
-      <c r="H5" s="3" t="str">
-        <f>$C$3&amp;"."&amp;G5</f>
-        <v>com.templengine.templatemanagement</v>
-      </c>
-      <c r="J5" s="3" t="str">
-        <f>H5&amp;".entity"</f>
-        <v>com.templengine.templatemanagement.entity</v>
-      </c>
-      <c r="K5" s="3" t="str">
-        <f>C5</f>
-        <v>Template</v>
-      </c>
-      <c r="M5" s="3" t="str">
-        <f>H5&amp;".dao"</f>
-        <v>com.templengine.templatemanagement.dao</v>
-      </c>
-      <c r="N5" s="3" t="str">
-        <f>C5&amp;"Dao"</f>
-        <v>TemplateDao</v>
-      </c>
-      <c r="P5" s="3" t="str">
-        <f>M5&amp;".mapper"</f>
-        <v>com.templengine.templatemanagement.dao.mapper</v>
-      </c>
-      <c r="Q5" s="3" t="str">
-        <f>K5&amp;"Mapper"</f>
-        <v>TemplateMapper</v>
-      </c>
-      <c r="S5" s="3" t="str">
-        <f>M5&amp;".mapper.gen"</f>
-        <v>com.templengine.templatemanagement.dao.mapper.gen</v>
-      </c>
-      <c r="T5" s="3" t="str">
-        <f>K5&amp;"MapperGen"</f>
-        <v>TemplateMapperGen</v>
-      </c>
-      <c r="V5" t="s">
-        <v>279</v>
-      </c>
-      <c r="W5" s="7" t="str">
-        <f>"/"&amp;LOWER(B5)&amp;V5</f>
-        <v>/templatemanagement/templates</v>
-      </c>
-      <c r="X5" s="3" t="str">
-        <f>H5&amp;".api"</f>
-        <v>com.templengine.templatemanagement.api</v>
-      </c>
-      <c r="Y5" s="3" t="str">
-        <f>C5&amp;"Api"</f>
-        <v>TemplateApi</v>
-      </c>
+      <c r="B5" s="9"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="C6" t="s">
-        <v>278</v>
-      </c>
-      <c r="E6" s="4" t="str">
-        <f t="shared" ref="E6" si="0">C6</f>
-        <v>TemplateParameter</v>
-      </c>
-      <c r="G6" s="3" t="str">
-        <f t="shared" ref="G6" si="1">LOWER(B6)</f>
-        <v>templatemanagement</v>
-      </c>
-      <c r="H6" s="3" t="str">
-        <f t="shared" ref="H6" si="2">$C$3&amp;"."&amp;G6</f>
-        <v>com.templengine.templatemanagement</v>
-      </c>
-      <c r="J6" s="3" t="str">
-        <f t="shared" ref="J6" si="3">H6&amp;".entity"</f>
-        <v>com.templengine.templatemanagement.entity</v>
-      </c>
-      <c r="K6" s="3" t="str">
-        <f t="shared" ref="K6" si="4">C6</f>
-        <v>TemplateParameter</v>
-      </c>
-      <c r="M6" s="3" t="str">
-        <f t="shared" ref="M6" si="5">H6&amp;".dao"</f>
-        <v>com.templengine.templatemanagement.dao</v>
-      </c>
-      <c r="N6" s="3" t="str">
-        <f t="shared" ref="N6" si="6">C6&amp;"Dao"</f>
-        <v>TemplateParameterDao</v>
-      </c>
-      <c r="P6" s="3" t="str">
-        <f t="shared" ref="P6" si="7">M6&amp;".mapper"</f>
-        <v>com.templengine.templatemanagement.dao.mapper</v>
-      </c>
-      <c r="Q6" s="3" t="str">
-        <f t="shared" ref="Q6" si="8">K6&amp;"Mapper"</f>
-        <v>TemplateParameterMapper</v>
-      </c>
-      <c r="S6" s="3" t="str">
-        <f t="shared" ref="S6" si="9">M6&amp;".mapper.gen"</f>
-        <v>com.templengine.templatemanagement.dao.mapper.gen</v>
-      </c>
-      <c r="T6" s="3" t="str">
-        <f t="shared" ref="T6" si="10">K6&amp;"MapperGen"</f>
-        <v>TemplateParameterMapperGen</v>
-      </c>
-      <c r="V6" t="s">
-        <v>280</v>
-      </c>
-      <c r="W6" s="7" t="str">
-        <f t="shared" ref="W6" si="11">"/"&amp;LOWER(B6)&amp;V6</f>
-        <v>/templatemanagement/templates/{templateId}/parameters</v>
-      </c>
-      <c r="X6" s="3" t="str">
-        <f t="shared" ref="X6" si="12">H6&amp;".api"</f>
-        <v>com.templengine.templatemanagement.api</v>
-      </c>
-      <c r="Y6" s="3" t="str">
-        <f t="shared" ref="Y6" si="13">C6&amp;"Api"</f>
-        <v>TemplateParameterApi</v>
-      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="9"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="J7" s="3"/>
@@ -3859,34 +3871,6 @@
       <c r="T8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -4075,7 +4059,7 @@
         <v>287</v>
       </c>
       <c r="B3" s="3" t="str">
-        <f>INDEX(Entities!$B$5:$B$7,MATCH(EntityProperties!C3,Entities!$C$5:$C$7,0))</f>
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C3,Entities!$C$3:$C$5,0))</f>
         <v>TemplateManagement</v>
       </c>
       <c r="C3" t="s">
@@ -4136,7 +4120,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3" t="str">
-        <f>INDEX(Entities!$B$5:$B$7,MATCH(EntityProperties!C4,Entities!$C$5:$C$7,0))</f>
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C4,Entities!$C$3:$C$5,0))</f>
         <v>TemplateManagement</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -4194,7 +4178,7 @@
     </row>
     <row r="5" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="3" t="str">
-        <f>INDEX(Entities!$B$5:$B$7,MATCH(EntityProperties!C5,Entities!$C$5:$C$7,0))</f>
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C5,Entities!$C$3:$C$5,0))</f>
         <v>TemplateManagement</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -4252,7 +4236,7 @@
     </row>
     <row r="6" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="3" t="str">
-        <f>INDEX(Entities!$B$5:$B$7,MATCH(EntityProperties!C6,Entities!$C$5:$C$7,0))</f>
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C6,Entities!$C$3:$C$5,0))</f>
         <v>TemplateManagement</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -4310,7 +4294,7 @@
     </row>
     <row r="7" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="3" t="str">
-        <f>INDEX(Entities!$B$5:$B$7,MATCH(EntityProperties!C7,Entities!$C$5:$C$7,0))</f>
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C7,Entities!$C$3:$C$5,0))</f>
         <v>TemplateManagement</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4368,7 +4352,7 @@
     </row>
     <row r="8" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="3" t="str">
-        <f>INDEX(Entities!$B$5:$B$7,MATCH(EntityProperties!C8,Entities!$C$5:$C$7,0))</f>
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C8,Entities!$C$3:$C$5,0))</f>
         <v>TemplateManagement</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -4426,7 +4410,7 @@
     </row>
     <row r="9" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="3" t="str">
-        <f>INDEX(Entities!$B$5:$B$7,MATCH(EntityProperties!C9,Entities!$C$5:$C$7,0))</f>
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C9,Entities!$C$3:$C$5,0))</f>
         <v>TemplateManagement</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -4484,7 +4468,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="3" t="str">
-        <f>INDEX(Entities!$B$5:$B$7,MATCH(EntityProperties!C10,Entities!$C$5:$C$7,0))</f>
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C10,Entities!$C$3:$C$5,0))</f>
         <v>TemplateManagement</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -4545,7 +4529,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="3" t="str">
-        <f>INDEX(Entities!$B$5:$B$7,MATCH(EntityProperties!C11,Entities!$C$5:$C$7,0))</f>
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C11,Entities!$C$3:$C$5,0))</f>
         <v>TemplateManagement</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -4606,7 +4590,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="3" t="str">
-        <f>INDEX(Entities!$B$5:$B$7,MATCH(EntityProperties!C12,Entities!$C$5:$C$7,0))</f>
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C12,Entities!$C$3:$C$5,0))</f>
         <v>TemplateManagement</v>
       </c>
       <c r="C12" s="9" t="s">

</xml_diff>

<commit_message>
Added templates for entity, mapperGen and mapperGen_xml
</commit_message>
<xml_diff>
--- a/template/AppDefinition.xlsx
+++ b/template/AppDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xltemplating\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC854A7F-E332-4B06-AA03-8A1D1ABA39FC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B790F043-DFF5-4C53-818B-5A25C6E729B5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Database-Entity'!$D$3:$D$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">DefaultEntityProperties!$A$1:$AD$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EntityProperties!$A$1:$AD$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EntityProperties!$A$1:$AD$6</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="322">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -494,10 +494,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Link</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1053,47 +1049,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>TemplateManagement</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>Template</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>TemplateParameter</t>
-  </si>
-  <si>
-    <t>TemplateParameter</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/templates</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/templates/{templateId}/parameters</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>templateId</t>
-  </si>
-  <si>
-    <t>templateId</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>parameterId</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>parameterName</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>byte[]</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1199,38 +1154,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>path</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>content</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>sampleDataJsonStr</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>contentType</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>com.templengine</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Application Name</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1239,10 +1162,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>templatemanagement</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>application#~</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1268,6 +1187,38 @@
   </si>
   <si>
     <t>basePackage</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Log</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>org.xlbean</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LogReceiver</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/logs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Log</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>logId</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>log-receiver</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1724,7 +1675,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1738,44 +1689,44 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
       <c r="B3" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="C3" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D3" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C4" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="D4" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -3028,13 +2979,13 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q4" t="s">
         <v>81</v>
       </c>
       <c r="R4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3048,13 +2999,13 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q5" t="s">
         <v>81</v>
       </c>
       <c r="R5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3068,13 +3019,13 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q6" t="s">
         <v>81</v>
       </c>
       <c r="R6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3094,7 +3045,7 @@
         <v>81</v>
       </c>
       <c r="R7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3108,7 +3059,7 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q8" t="s">
         <v>81</v>
@@ -3128,13 +3079,13 @@
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q9" t="s">
         <v>81</v>
       </c>
       <c r="R9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3142,19 +3093,19 @@
         <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E10">
         <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q10" t="s">
         <v>81</v>
       </c>
       <c r="R10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3168,7 +3119,7 @@
         <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q11" t="s">
         <v>81</v>
@@ -3188,7 +3139,7 @@
         <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q12" t="s">
         <v>81</v>
@@ -3208,13 +3159,13 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q13" t="s">
         <v>111</v>
       </c>
       <c r="R13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3222,19 +3173,19 @@
         <v>112</v>
       </c>
       <c r="D14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="H14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q14" t="s">
         <v>111</v>
       </c>
       <c r="R14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3248,13 +3199,13 @@
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q15" t="s">
         <v>111</v>
       </c>
       <c r="R15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3268,7 +3219,7 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q16" t="s">
         <v>55</v>
@@ -3288,13 +3239,13 @@
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q17" t="s">
         <v>55</v>
       </c>
       <c r="R17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3308,13 +3259,13 @@
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q18" t="s">
         <v>55</v>
       </c>
       <c r="R18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3334,7 +3285,7 @@
         <v>55</v>
       </c>
       <c r="R19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3348,13 +3299,13 @@
         <v>6</v>
       </c>
       <c r="H20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q20" t="s">
         <v>55</v>
       </c>
       <c r="R20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3368,7 +3319,7 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q21" t="s">
         <v>100</v>
@@ -3382,19 +3333,19 @@
         <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E22">
         <v>2</v>
       </c>
       <c r="H22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q22" t="s">
         <v>100</v>
       </c>
       <c r="R22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3408,13 +3359,13 @@
         <v>3</v>
       </c>
       <c r="H23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q23" t="s">
         <v>100</v>
       </c>
       <c r="R23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3428,13 +3379,13 @@
         <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q24" t="s">
         <v>100</v>
       </c>
       <c r="R24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3448,13 +3399,13 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q25" t="s">
         <v>106</v>
       </c>
       <c r="R25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3468,7 +3419,7 @@
         <v>2</v>
       </c>
       <c r="H26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q26" t="s">
         <v>106</v>
@@ -3488,13 +3439,13 @@
         <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q27" t="s">
         <v>106</v>
       </c>
       <c r="R27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3508,13 +3459,13 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q28" t="s">
         <v>108</v>
       </c>
       <c r="R28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3528,7 +3479,7 @@
         <v>2</v>
       </c>
       <c r="H29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q29" t="s">
         <v>108</v>
@@ -3539,27 +3490,27 @@
     </row>
     <row r="30" spans="3:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" t="s">
         <v>139</v>
-      </c>
-      <c r="D30" t="s">
-        <v>140</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="R30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="3:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D31" t="s">
         <v>90</v>
@@ -3568,10 +3519,10 @@
         <v>2</v>
       </c>
       <c r="H31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="R31" t="s">
         <v>90</v>
@@ -3585,10 +3536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3622,201 +3573,148 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" t="s">
         <v>174</v>
       </c>
-      <c r="C1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>175</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M1" t="s">
         <v>176</v>
       </c>
-      <c r="J1" t="s">
-        <v>172</v>
-      </c>
-      <c r="K1" t="s">
-        <v>173</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>177</v>
       </c>
-      <c r="N1" t="s">
-        <v>178</v>
-      </c>
       <c r="P1" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q1" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="Q1" s="6" t="s">
-        <v>212</v>
-      </c>
       <c r="S1" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>242</v>
-      </c>
       <c r="W1" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="X1" t="s">
+        <v>243</v>
+      </c>
+      <c r="Y1" t="s">
         <v>244</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="V2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>274</v>
+        <v>316</v>
       </c>
       <c r="C3" t="s">
-        <v>276</v>
+        <v>314</v>
       </c>
       <c r="E3" s="4" t="str">
         <f>C3</f>
-        <v>Template</v>
+        <v>Log</v>
       </c>
       <c r="G3" s="3" t="str">
         <f>LOWER(B3)</f>
-        <v>templatemanagement</v>
+        <v>logreceiver</v>
       </c>
       <c r="H3" s="3" t="str">
         <f>Application!$D$5&amp;"."&amp;G3</f>
-        <v>com.templengine.templatemanagement</v>
+        <v>org.xlbean.logreceiver</v>
       </c>
       <c r="J3" s="3" t="str">
         <f>H3&amp;".entity"</f>
-        <v>com.templengine.templatemanagement.entity</v>
+        <v>org.xlbean.logreceiver.entity</v>
       </c>
       <c r="K3" s="3" t="str">
         <f>C3</f>
-        <v>Template</v>
+        <v>Log</v>
       </c>
       <c r="M3" s="3" t="str">
         <f>H3&amp;".dao"</f>
-        <v>com.templengine.templatemanagement.dao</v>
+        <v>org.xlbean.logreceiver.dao</v>
       </c>
       <c r="N3" s="3" t="str">
         <f>C3&amp;"Dao"</f>
-        <v>TemplateDao</v>
+        <v>LogDao</v>
       </c>
       <c r="P3" s="3" t="str">
         <f>M3&amp;".mapper"</f>
-        <v>com.templengine.templatemanagement.dao.mapper</v>
+        <v>org.xlbean.logreceiver.dao.mapper</v>
       </c>
       <c r="Q3" s="3" t="str">
         <f>K3&amp;"Mapper"</f>
-        <v>TemplateMapper</v>
+        <v>LogMapper</v>
       </c>
       <c r="S3" s="3" t="str">
         <f>M3&amp;".mapper.gen"</f>
-        <v>com.templengine.templatemanagement.dao.mapper.gen</v>
+        <v>org.xlbean.logreceiver.dao.mapper.gen</v>
       </c>
       <c r="T3" s="3" t="str">
         <f>K3&amp;"MapperGen"</f>
-        <v>TemplateMapperGen</v>
+        <v>LogMapperGen</v>
       </c>
       <c r="V3" t="s">
-        <v>279</v>
+        <v>317</v>
       </c>
       <c r="W3" s="7" t="str">
         <f>"/"&amp;LOWER(B3)&amp;V3</f>
-        <v>/templatemanagement/templates</v>
+        <v>/logreceiver/logs</v>
       </c>
       <c r="X3" s="3" t="str">
         <f>H3&amp;".api"</f>
-        <v>com.templengine.templatemanagement.api</v>
+        <v>org.xlbean.logreceiver.api</v>
       </c>
       <c r="Y3" s="3" t="str">
         <f>C3&amp;"Api"</f>
-        <v>TemplateApi</v>
+        <v>LogApi</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="C4" t="s">
-        <v>278</v>
-      </c>
-      <c r="E4" s="4" t="str">
-        <f t="shared" ref="E4" si="0">C4</f>
-        <v>TemplateParameter</v>
-      </c>
-      <c r="G4" s="3" t="str">
-        <f t="shared" ref="G4" si="1">LOWER(B4)</f>
-        <v>templatemanagement</v>
-      </c>
-      <c r="H4" s="3" t="str">
-        <f>Application!$D$5&amp;"."&amp;G4</f>
-        <v>com.templengine.templatemanagement</v>
-      </c>
-      <c r="J4" s="3" t="str">
-        <f t="shared" ref="J4" si="2">H4&amp;".entity"</f>
-        <v>com.templengine.templatemanagement.entity</v>
-      </c>
-      <c r="K4" s="3" t="str">
-        <f t="shared" ref="K4" si="3">C4</f>
-        <v>TemplateParameter</v>
-      </c>
-      <c r="M4" s="3" t="str">
-        <f t="shared" ref="M4" si="4">H4&amp;".dao"</f>
-        <v>com.templengine.templatemanagement.dao</v>
-      </c>
-      <c r="N4" s="3" t="str">
-        <f t="shared" ref="N4" si="5">C4&amp;"Dao"</f>
-        <v>TemplateParameterDao</v>
-      </c>
-      <c r="P4" s="3" t="str">
-        <f t="shared" ref="P4" si="6">M4&amp;".mapper"</f>
-        <v>com.templengine.templatemanagement.dao.mapper</v>
-      </c>
-      <c r="Q4" s="3" t="str">
-        <f t="shared" ref="Q4" si="7">K4&amp;"Mapper"</f>
-        <v>TemplateParameterMapper</v>
-      </c>
-      <c r="S4" s="3" t="str">
-        <f t="shared" ref="S4" si="8">M4&amp;".mapper.gen"</f>
-        <v>com.templengine.templatemanagement.dao.mapper.gen</v>
-      </c>
-      <c r="T4" s="3" t="str">
-        <f t="shared" ref="T4" si="9">K4&amp;"MapperGen"</f>
-        <v>TemplateParameterMapperGen</v>
-      </c>
-      <c r="V4" t="s">
-        <v>280</v>
-      </c>
-      <c r="W4" s="7" t="str">
-        <f t="shared" ref="W4" si="10">"/"&amp;LOWER(B4)&amp;V4</f>
-        <v>/templatemanagement/templates/{templateId}/parameters</v>
-      </c>
-      <c r="X4" s="3" t="str">
-        <f t="shared" ref="X4" si="11">H4&amp;".api"</f>
-        <v>com.templengine.templatemanagement.api</v>
-      </c>
-      <c r="Y4" s="3" t="str">
-        <f t="shared" ref="Y4" si="12">C4&amp;"Api"</f>
-        <v>TemplateParameterApi</v>
-      </c>
+      <c r="B4" s="9"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="9"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="J5" s="3"/>
@@ -3858,20 +3756,6 @@
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3881,10 +3765,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD17"/>
+  <dimension ref="A1:AD9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -3908,90 +3792,90 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C1" t="s">
         <v>117</v>
       </c>
       <c r="D1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K1" t="s">
         <v>187</v>
       </c>
-      <c r="E1" t="s">
-        <v>243</v>
-      </c>
-      <c r="F1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>188</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>189</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>303</v>
+      </c>
+      <c r="O1" t="s">
         <v>190</v>
       </c>
-      <c r="N1" t="s">
-        <v>315</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>191</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>192</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>193</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>194</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>195</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>196</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>197</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>198</v>
       </c>
-      <c r="W1" t="s">
-        <v>199</v>
-      </c>
       <c r="Y1" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>267</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="AD1" s="8" t="s">
         <v>272</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>268</v>
-      </c>
-      <c r="AA1" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="AD1" s="8" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
         <v>83</v>
@@ -4009,64 +3893,64 @@
         <v>119</v>
       </c>
       <c r="H2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L2" t="s">
+        <v>247</v>
+      </c>
+      <c r="M2" t="s">
         <v>249</v>
       </c>
-      <c r="L2" t="s">
-        <v>248</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>250</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>251</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>252</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>253</v>
       </c>
-      <c r="R2" t="s">
+      <c r="V2" t="s">
         <v>254</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="Z2" t="s">
         <v>255</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="AA2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB2" t="s">
         <v>259</v>
       </c>
-      <c r="Z2" t="s">
-        <v>256</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>257</v>
-      </c>
-      <c r="AB2" t="s">
+      <c r="AC2" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="AC2" s="8" t="s">
-        <v>261</v>
-      </c>
       <c r="AD2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="B3" s="3" t="str">
-        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C3,Entities!$C$3:$C$5,0))</f>
-        <v>TemplateManagement</v>
+        <f>INDEX(Entities!$B$3:$B$4,MATCH(EntityProperties!C3,Entities!$C$3:$C$4,0))</f>
+        <v>LogReceiver</v>
       </c>
       <c r="C3" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="D3" t="s">
-        <v>282</v>
+        <v>319</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -4079,15 +3963,15 @@
       </c>
       <c r="K3" s="3" t="str">
         <f>UPPER(B3)</f>
-        <v>TEMPLATEMANAGEMENT</v>
+        <v>LOGRECEIVER</v>
       </c>
       <c r="L3" s="3" t="str">
         <f>VLOOKUP(C3,Entities!C:E,3,FALSE)</f>
-        <v>Template</v>
+        <v>Log</v>
       </c>
       <c r="M3" s="3" t="str">
         <f>D3</f>
-        <v>templateId</v>
+        <v>logId</v>
       </c>
       <c r="N3" s="3">
         <f>IF(L3=L2,N2+1,1)</f>
@@ -4120,39 +4004,39 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3" t="str">
-        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C4,Entities!$C$3:$C$5,0))</f>
-        <v>TemplateManagement</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>275</v>
+        <f>INDEX(Entities!$B$3:$B$4,MATCH(EntityProperties!C4,Entities!$C$3:$C$4,0))</f>
+        <v>LogReceiver</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>318</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="F4" t="s">
         <v>123</v>
       </c>
       <c r="G4">
-        <v>128</v>
+        <v>1000000</v>
       </c>
       <c r="K4" s="3" t="str">
         <f t="shared" ref="K4" si="0">UPPER(B4)</f>
-        <v>TEMPLATEMANAGEMENT</v>
+        <v>LOGRECEIVER</v>
       </c>
       <c r="L4" s="3" t="str">
         <f>VLOOKUP(C4,Entities!C:E,3,FALSE)</f>
-        <v>Template</v>
+        <v>Log</v>
       </c>
       <c r="M4" s="3" t="str">
         <f t="shared" ref="M4" si="1">D4</f>
-        <v>name</v>
+        <v>data</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" ref="N4" si="2">IF(L4=L3,N3+1,1)</f>
         <v>2</v>
       </c>
       <c r="P4" s="6" t="str">
-        <f t="shared" ref="P4:P12" si="3">IF(E4=1,"NO","YES")</f>
+        <f t="shared" ref="P4" si="3">IF(E4=1,"NO","YES")</f>
         <v>YES</v>
       </c>
       <c r="Q4" s="3" t="str">
@@ -4160,585 +4044,114 @@
         <v>varchar</v>
       </c>
       <c r="R4" s="3">
-        <f t="shared" ref="R4:R12" si="4">IF(OR(Q4="char",Q4="varchar"),IF(G4="-",50,G4),IF(Q4="int",11,""))</f>
-        <v>128</v>
+        <f t="shared" ref="R4" si="4">IF(OR(Q4="char",Q4="varchar"),IF(G4="-",50,G4),IF(Q4="int",11,""))</f>
+        <v>1000000</v>
       </c>
       <c r="V4" s="3" t="str">
-        <f t="shared" ref="V4:V12" si="5">IF(R4="",Q4,Q4&amp;"("&amp;R4&amp;")")</f>
-        <v>varchar(128)</v>
+        <f t="shared" ref="V4" si="5">IF(R4="",Q4,Q4&amp;"("&amp;R4&amp;")")</f>
+        <v>varchar(1000000)</v>
       </c>
       <c r="Y4" s="8" t="str">
-        <f t="shared" ref="Y4:Y17" si="6">IF(E4&lt;&gt;"","NotNull","")</f>
+        <f t="shared" ref="Y4:Y9" si="6">IF(E4&lt;&gt;"","NotNull","")</f>
         <v/>
       </c>
       <c r="AC4">
-        <f t="shared" ref="AC4:AC17" si="7">IF(G4&lt;&gt;"-",G4,"")</f>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="3" t="str">
-        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C5,Entities!$C$3:$C$5,0))</f>
-        <v>TemplateManagement</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="11">
-        <v>1024</v>
-      </c>
-      <c r="K5" s="3" t="str">
-        <f t="shared" ref="K5:K6" si="8">UPPER(B5)</f>
-        <v>TEMPLATEMANAGEMENT</v>
-      </c>
-      <c r="L5" s="3" t="str">
-        <f>VLOOKUP(C5,Entities!C:E,3,FALSE)</f>
-        <v>Template</v>
-      </c>
-      <c r="M5" s="3" t="str">
-        <f t="shared" ref="M5:M6" si="9">D5</f>
-        <v>description</v>
-      </c>
-      <c r="N5" s="3">
-        <f t="shared" ref="N5:N6" si="10">IF(L5=L4,N4+1,1)</f>
-        <v>3</v>
-      </c>
-      <c r="P5" s="11" t="str">
-        <f t="shared" ref="P5:P6" si="11">IF(E5=1,"NO","YES")</f>
-        <v>YES</v>
-      </c>
-      <c r="Q5" s="3" t="str">
-        <f>VLOOKUP(F5,vlookup!$B:$C,2,FALSE)</f>
-        <v>varchar</v>
-      </c>
-      <c r="R5" s="3">
-        <f t="shared" ref="R5:R6" si="12">IF(OR(Q5="char",Q5="varchar"),IF(G5="-",50,G5),IF(Q5="int",11,""))</f>
-        <v>1024</v>
-      </c>
-      <c r="V5" s="3" t="str">
-        <f t="shared" ref="V5:V6" si="13">IF(R5="",Q5,Q5&amp;"("&amp;R5&amp;")")</f>
-        <v>varchar(1024)</v>
-      </c>
-      <c r="Y5" s="11" t="str">
-        <f t="shared" ref="Y5:Y6" si="14">IF(E5&lt;&gt;"","NotNull","")</f>
-        <v/>
-      </c>
-      <c r="AC5" s="11">
-        <f t="shared" ref="AC5:AC6" si="15">IF(G5&lt;&gt;"-",G5,"")</f>
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="3" t="str">
-        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C6,Entities!$C$3:$C$5,0))</f>
-        <v>TemplateManagement</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="G6" s="11">
-        <v>512</v>
-      </c>
-      <c r="K6" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>TEMPLATEMANAGEMENT</v>
-      </c>
-      <c r="L6" s="3" t="str">
-        <f>VLOOKUP(C6,Entities!C:E,3,FALSE)</f>
-        <v>Template</v>
-      </c>
-      <c r="M6" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v>path</v>
-      </c>
-      <c r="N6" s="3">
-        <f t="shared" si="10"/>
-        <v>4</v>
-      </c>
-      <c r="P6" s="11" t="str">
-        <f t="shared" si="11"/>
-        <v>YES</v>
-      </c>
-      <c r="Q6" s="3" t="str">
-        <f>VLOOKUP(F6,vlookup!$B:$C,2,FALSE)</f>
-        <v>varchar</v>
-      </c>
-      <c r="R6" s="3">
-        <f t="shared" si="12"/>
-        <v>512</v>
-      </c>
-      <c r="V6" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>varchar(512)</v>
-      </c>
-      <c r="Y6" s="11" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="AC6" s="11">
-        <f t="shared" si="15"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="3" t="str">
-        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C7,Entities!$C$3:$C$5,0))</f>
-        <v>TemplateManagement</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="G7" s="11">
+        <f t="shared" ref="AC4:AC9" si="7">IF(G4&lt;&gt;"-",G4,"")</f>
         <v>1000000</v>
       </c>
-      <c r="K7" s="3" t="str">
-        <f t="shared" ref="K7" si="16">UPPER(B7)</f>
-        <v>TEMPLATEMANAGEMENT</v>
-      </c>
-      <c r="L7" s="3" t="str">
-        <f>VLOOKUP(C7,Entities!C:E,3,FALSE)</f>
-        <v>Template</v>
-      </c>
-      <c r="M7" s="3" t="str">
-        <f t="shared" ref="M7" si="17">D7</f>
-        <v>content</v>
-      </c>
-      <c r="N7" s="3">
-        <f t="shared" ref="N7:N12" si="18">IF(L7=L6,N6+1,1)</f>
-        <v>5</v>
-      </c>
-      <c r="P7" s="11" t="str">
-        <f t="shared" ref="P7" si="19">IF(E7=1,"NO","YES")</f>
-        <v>YES</v>
-      </c>
-      <c r="Q7" s="3" t="str">
-        <f>VLOOKUP(F7,vlookup!$B:$C,2,FALSE)</f>
-        <v>varchar</v>
-      </c>
-      <c r="R7" s="3">
-        <f t="shared" ref="R7" si="20">IF(OR(Q7="char",Q7="varchar"),IF(G7="-",50,G7),IF(Q7="int",11,""))</f>
-        <v>1000000</v>
-      </c>
-      <c r="V7" s="3" t="str">
-        <f t="shared" ref="V7" si="21">IF(R7="",Q7,Q7&amp;"("&amp;R7&amp;")")</f>
-        <v>varchar(1000000)</v>
-      </c>
-      <c r="Y7" s="11" t="str">
-        <f t="shared" ref="Y7" si="22">IF(E7&lt;&gt;"","NotNull","")</f>
-        <v/>
-      </c>
-      <c r="AC7" s="11">
-        <f t="shared" ref="AC7" si="23">IF(G7&lt;&gt;"-",G7,"")</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="3" t="str">
-        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C8,Entities!$C$3:$C$5,0))</f>
-        <v>TemplateManagement</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="G8" s="11">
-        <v>20</v>
-      </c>
-      <c r="K8" s="3" t="str">
-        <f t="shared" ref="K8" si="24">UPPER(B8)</f>
-        <v>TEMPLATEMANAGEMENT</v>
-      </c>
-      <c r="L8" s="3" t="str">
-        <f>VLOOKUP(C8,Entities!C:E,3,FALSE)</f>
-        <v>Template</v>
-      </c>
-      <c r="M8" s="3" t="str">
-        <f t="shared" ref="M8" si="25">D8</f>
-        <v>contentType</v>
-      </c>
-      <c r="N8" s="3">
-        <f t="shared" ref="N8" si="26">IF(L8=L7,N7+1,1)</f>
-        <v>6</v>
-      </c>
-      <c r="P8" s="11" t="str">
-        <f t="shared" ref="P8" si="27">IF(E8=1,"NO","YES")</f>
-        <v>YES</v>
-      </c>
-      <c r="Q8" s="3" t="str">
-        <f>VLOOKUP(F8,vlookup!$B:$C,2,FALSE)</f>
-        <v>varchar</v>
-      </c>
-      <c r="R8" s="3">
-        <f t="shared" ref="R8" si="28">IF(OR(Q8="char",Q8="varchar"),IF(G8="-",50,G8),IF(Q8="int",11,""))</f>
-        <v>20</v>
-      </c>
-      <c r="V8" s="3" t="str">
-        <f t="shared" ref="V8" si="29">IF(R8="",Q8,Q8&amp;"("&amp;R8&amp;")")</f>
-        <v>varchar(20)</v>
-      </c>
-      <c r="Y8" s="11" t="str">
-        <f t="shared" ref="Y8" si="30">IF(E8&lt;&gt;"","NotNull","")</f>
-        <v/>
-      </c>
-      <c r="AC8" s="11">
-        <f t="shared" ref="AC8" si="31">IF(G8&lt;&gt;"-",G8,"")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="3" t="str">
-        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C9,Entities!$C$3:$C$5,0))</f>
-        <v>TemplateManagement</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>322</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="G9" s="11">
-        <v>10000</v>
-      </c>
-      <c r="K9" s="3" t="str">
-        <f t="shared" ref="K9" si="32">UPPER(B9)</f>
-        <v>TEMPLATEMANAGEMENT</v>
-      </c>
-      <c r="L9" s="3" t="str">
-        <f>VLOOKUP(C9,Entities!C:E,3,FALSE)</f>
-        <v>Template</v>
-      </c>
-      <c r="M9" s="3" t="str">
-        <f t="shared" ref="M9" si="33">D9</f>
-        <v>sampleDataJsonStr</v>
-      </c>
-      <c r="N9" s="3">
-        <f t="shared" ref="N9" si="34">IF(L9=L7,N7+1,1)</f>
-        <v>6</v>
-      </c>
-      <c r="P9" s="11" t="str">
-        <f t="shared" ref="P9" si="35">IF(E9=1,"NO","YES")</f>
-        <v>YES</v>
-      </c>
-      <c r="Q9" s="3" t="str">
-        <f>VLOOKUP(F9,vlookup!$B:$C,2,FALSE)</f>
-        <v>varchar</v>
-      </c>
-      <c r="R9" s="3">
-        <f t="shared" ref="R9" si="36">IF(OR(Q9="char",Q9="varchar"),IF(G9="-",50,G9),IF(Q9="int",11,""))</f>
-        <v>10000</v>
-      </c>
-      <c r="V9" s="3" t="str">
-        <f t="shared" ref="V9" si="37">IF(R9="",Q9,Q9&amp;"("&amp;R9&amp;")")</f>
-        <v>varchar(10000)</v>
-      </c>
-      <c r="Y9" s="11" t="str">
-        <f t="shared" ref="Y9" si="38">IF(E9&lt;&gt;"","NotNull","")</f>
-        <v/>
-      </c>
-      <c r="AC9" s="11">
-        <f t="shared" ref="AC9" si="39">IF(G9&lt;&gt;"-",G9,"")</f>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="3" t="str">
-        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C10,Entities!$C$3:$C$5,0))</f>
-        <v>TemplateManagement</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="D10" t="s">
-        <v>281</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>120</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="K10" s="3" t="str">
-        <f t="shared" ref="K10:K12" si="40">UPPER(B10)</f>
-        <v>TEMPLATEMANAGEMENT</v>
-      </c>
-      <c r="L10" s="3" t="str">
-        <f>VLOOKUP(C10,Entities!C:E,3,FALSE)</f>
-        <v>TemplateParameter</v>
-      </c>
-      <c r="M10" s="3" t="str">
-        <f t="shared" ref="M10:M12" si="41">D10</f>
-        <v>templateId</v>
-      </c>
-      <c r="N10" s="3">
-        <f>IF(L10=L7,N7+1,1)</f>
-        <v>1</v>
-      </c>
-      <c r="P10" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>NO</v>
-      </c>
-      <c r="Q10" s="3" t="str">
-        <f>VLOOKUP(F10,vlookup!$B:$C,2,FALSE)</f>
-        <v>int</v>
-      </c>
-      <c r="R10" s="3">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="V10" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>int(11)</v>
-      </c>
-      <c r="Y10" s="8" t="str">
-        <f t="shared" si="6"/>
-        <v>NotNull</v>
-      </c>
-      <c r="AC10" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="3" t="str">
-        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C11,Entities!$C$3:$C$5,0))</f>
-        <v>TemplateManagement</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="G11" t="s">
-        <v>128</v>
-      </c>
-      <c r="K11" s="3" t="str">
-        <f t="shared" si="40"/>
-        <v>TEMPLATEMANAGEMENT</v>
-      </c>
-      <c r="L11" s="3" t="str">
-        <f>VLOOKUP(C11,Entities!C:E,3,FALSE)</f>
-        <v>TemplateParameter</v>
-      </c>
-      <c r="M11" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>parameterId</v>
-      </c>
-      <c r="N11" s="3">
-        <f t="shared" si="18"/>
-        <v>2</v>
-      </c>
-      <c r="P11" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>YES</v>
-      </c>
-      <c r="Q11" s="3" t="str">
-        <f>VLOOKUP(F11,vlookup!$B:$C,2,FALSE)</f>
-        <v>int</v>
-      </c>
-      <c r="R11" s="3">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="V11" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>int(11)</v>
-      </c>
-      <c r="Y11" s="8" t="str">
-        <f t="shared" si="6"/>
-        <v>NotNull</v>
-      </c>
-      <c r="AC11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="3" t="str">
-        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C12,Entities!$C$3:$C$5,0))</f>
-        <v>TemplateManagement</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="D12" t="s">
-        <v>284</v>
-      </c>
-      <c r="F12" t="s">
-        <v>123</v>
-      </c>
-      <c r="G12">
-        <v>255</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="K12" s="3" t="str">
-        <f t="shared" si="40"/>
-        <v>TEMPLATEMANAGEMENT</v>
-      </c>
-      <c r="L12" s="3" t="str">
-        <f>VLOOKUP(C12,Entities!C:E,3,FALSE)</f>
-        <v>TemplateParameter</v>
-      </c>
-      <c r="M12" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>parameterName</v>
-      </c>
-      <c r="N12" s="3">
-        <f t="shared" si="18"/>
-        <v>3</v>
-      </c>
-      <c r="P12" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>YES</v>
-      </c>
-      <c r="Q12" s="3" t="str">
-        <f>VLOOKUP(F12,vlookup!$B:$C,2,FALSE)</f>
-        <v>varchar</v>
-      </c>
-      <c r="R12" s="3">
-        <f t="shared" si="4"/>
-        <v>255</v>
-      </c>
-      <c r="V12" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>varchar(255)</v>
-      </c>
-      <c r="Y12" s="8" t="str">
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="3"/>
+      <c r="C5" s="9"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="V5" s="3"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="3"/>
+      <c r="C6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="V6" s="3"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="Y7" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AC12">
+      <c r="AC7">
         <f t="shared" si="7"/>
-        <v>255</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="3"/>
-      <c r="C13" s="9"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="V13" s="3"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="3"/>
-      <c r="C14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="V14" s="3"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="Y15" s="8" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="Y8" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AC15">
+      <c r="AC8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="Y16" s="8" t="str">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="Y9" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AC16">
+      <c r="AC9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="Y17" s="8" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="AC17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:AD14" xr:uid="{B02FBA99-861D-4255-8BEE-D719BA83889D}"/>
+  <autoFilter ref="A1:AD6" xr:uid="{B02FBA99-861D-4255-8BEE-D719BA83889D}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="Z3:AA17">
+  <conditionalFormatting sqref="Z3:AA9">
     <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND($F3&lt;&gt;"Integer")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AD17">
+  <conditionalFormatting sqref="AB3:AD9">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>NOT($F3="String")</formula>
     </cfRule>
@@ -4752,13 +4165,13 @@
           <x14:formula1>
             <xm:f>List!$B$2:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>Y3:Y17</xm:sqref>
+          <xm:sqref>Y3:Y9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B0F9129-3A24-4315-8826-417A47D2DED6}">
           <x14:formula1>
             <xm:f>vlookup!$B$2:$B$20</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F17</xm:sqref>
+          <xm:sqref>F3:F9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4799,78 +4212,78 @@
         <v>0</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="T1" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="V1" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="W1" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="Y1" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="N1" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="O1" s="10" t="s">
+      <c r="AB1" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="AC1" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="AD1" s="10" t="s">
         <v>297</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="W1" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>307</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="AD1" s="10" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>83</v>
@@ -4888,10 +4301,10 @@
         <v>119</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>53</v>
@@ -4900,7 +4313,7 @@
         <v>54</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P2" s="10" t="s">
         <v>58</v>
@@ -4915,35 +4328,35 @@
         <v>65</v>
       </c>
       <c r="Y2" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB2" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="Z2" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="AA2" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="AB2" s="10" t="s">
+      <c r="AC2" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="AC2" s="10" t="s">
-        <v>261</v>
-      </c>
       <c r="AD2" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="10" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="10" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>72</v>
@@ -4989,7 +4402,7 @@
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="10" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>123</v>
@@ -5039,10 +4452,10 @@
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="10" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>72</v>
@@ -5089,7 +4502,7 @@
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="10" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>123</v>
@@ -5255,74 +4668,74 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
         <v>141</v>
-      </c>
-      <c r="D1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
         <v>134</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>135</v>
-      </c>
-      <c r="D2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" t="s">
         <v>206</v>
       </c>
-      <c r="C5" t="s">
-        <v>207</v>
-      </c>
       <c r="D5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -5353,92 +4766,92 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>227</v>
-      </c>
       <c r="L1" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H2" t="s">
         <v>236</v>
       </c>
-      <c r="G2" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>240</v>
-      </c>
       <c r="L2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H3" t="s">
         <v>95</v>
       </c>
       <c r="L3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -5446,16 +4859,16 @@
         <v>82</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G4" t="s">
         <v>112</v>
       </c>
       <c r="H4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -5481,15 +4894,15 @@
   <sheetData>
     <row r="1" spans="2:3" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" t="s">
         <v>182</v>
-      </c>
-      <c r="C2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
@@ -5497,15 +4910,15 @@
         <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
@@ -5513,7 +4926,7 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
@@ -5521,7 +4934,7 @@
         <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.55000000000000004">
@@ -5529,15 +4942,15 @@
         <v>122</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="C8" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -5562,25 +4975,25 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated build.gradle for templates
</commit_message>
<xml_diff>
--- a/template/AppDefinition.xlsx
+++ b/template/AppDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xltemplating\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B790F043-DFF5-4C53-818B-5A25C6E729B5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7CBAB8-DA8D-4ADD-9A55-56566C67CDD7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Database-Entity'!$D$3:$D$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">DefaultEntityProperties!$A$1:$AD$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EntityProperties!$A$1:$AD$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EntityProperties!$A$1:$AD$14</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="335">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -494,6 +494,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>Link</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1049,6 +1053,47 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>TemplateManagement</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>Template</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TemplateParameter</t>
+  </si>
+  <si>
+    <t>TemplateParameter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/templates</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/templates/{templateId}/parameters</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>templateId</t>
+  </si>
+  <si>
+    <t>templateId</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>parameterId</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>parameterName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>byte[]</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1154,6 +1199,38 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>path</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sampleDataJsonStr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>contentType</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>com.templengine</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>Application Name</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1162,6 +1239,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>templatemanagement</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>application#~</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1174,14 +1255,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>application#key?listToPropKey=true</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>application#value?listToPropValue=true</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>.xtmpl</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1190,35 +1263,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Log</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>org.xlbean</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>LogReceiver</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/logs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Log</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>logId</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>data</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>log-receiver</t>
+    <t>application#key?listToProp=key</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>application#value?listToProp=value</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1675,7 +1724,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1689,44 +1738,44 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>310</v>
+        <v>333</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>307</v>
+        <v>328</v>
       </c>
       <c r="B3" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="C3" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D3" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
-        <v>309</v>
+        <v>330</v>
       </c>
       <c r="C4" t="s">
-        <v>308</v>
+        <v>329</v>
       </c>
       <c r="D4" t="s">
-        <v>312</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" t="s">
-        <v>313</v>
+        <v>332</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -2979,13 +3028,13 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="Q4" t="s">
         <v>81</v>
       </c>
       <c r="R4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -2999,13 +3048,13 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="Q5" t="s">
         <v>81</v>
       </c>
       <c r="R5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3019,13 +3068,13 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="Q6" t="s">
         <v>81</v>
       </c>
       <c r="R6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3045,7 +3094,7 @@
         <v>81</v>
       </c>
       <c r="R7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3059,7 +3108,7 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="Q8" t="s">
         <v>81</v>
@@ -3079,13 +3128,13 @@
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="Q9" t="s">
         <v>81</v>
       </c>
       <c r="R9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3093,19 +3142,19 @@
         <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E10">
         <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="Q10" t="s">
         <v>81</v>
       </c>
       <c r="R10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3119,7 +3168,7 @@
         <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="Q11" t="s">
         <v>81</v>
@@ -3139,7 +3188,7 @@
         <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="Q12" t="s">
         <v>81</v>
@@ -3159,13 +3208,13 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q13" t="s">
         <v>111</v>
       </c>
       <c r="R13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3173,19 +3222,19 @@
         <v>112</v>
       </c>
       <c r="D14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="H14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Q14" t="s">
         <v>111</v>
       </c>
       <c r="R14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3199,13 +3248,13 @@
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q15" t="s">
         <v>111</v>
       </c>
       <c r="R15" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.55000000000000004">
@@ -3219,7 +3268,7 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q16" t="s">
         <v>55</v>
@@ -3239,13 +3288,13 @@
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Q17" t="s">
         <v>55</v>
       </c>
       <c r="R17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3259,13 +3308,13 @@
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="Q18" t="s">
         <v>55</v>
       </c>
       <c r="R18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3285,7 +3334,7 @@
         <v>55</v>
       </c>
       <c r="R19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3299,13 +3348,13 @@
         <v>6</v>
       </c>
       <c r="H20" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q20" t="s">
         <v>55</v>
       </c>
       <c r="R20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3319,7 +3368,7 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q21" t="s">
         <v>100</v>
@@ -3333,19 +3382,19 @@
         <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E22">
         <v>2</v>
       </c>
       <c r="H22" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q22" t="s">
         <v>100</v>
       </c>
       <c r="R22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3359,13 +3408,13 @@
         <v>3</v>
       </c>
       <c r="H23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q23" t="s">
         <v>100</v>
       </c>
       <c r="R23" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3379,13 +3428,13 @@
         <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q24" t="s">
         <v>100</v>
       </c>
       <c r="R24" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3399,13 +3448,13 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q25" t="s">
         <v>106</v>
       </c>
       <c r="R25" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3419,7 +3468,7 @@
         <v>2</v>
       </c>
       <c r="H26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="Q26" t="s">
         <v>106</v>
@@ -3439,13 +3488,13 @@
         <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q27" t="s">
         <v>106</v>
       </c>
       <c r="R27" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3459,13 +3508,13 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q28" t="s">
         <v>108</v>
       </c>
       <c r="R28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="3:18" x14ac:dyDescent="0.55000000000000004">
@@ -3479,7 +3528,7 @@
         <v>2</v>
       </c>
       <c r="H29" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="Q29" t="s">
         <v>108</v>
@@ -3490,27 +3539,27 @@
     </row>
     <row r="30" spans="3:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R30" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="3:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C31" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D31" t="s">
         <v>90</v>
@@ -3519,10 +3568,10 @@
         <v>2</v>
       </c>
       <c r="H31" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="Q31" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R31" t="s">
         <v>90</v>
@@ -3536,10 +3585,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z7"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" outlineLevelCol="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3573,148 +3622,201 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" t="s">
         <v>173</v>
       </c>
-      <c r="C1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="M1" t="s">
+        <v>177</v>
+      </c>
+      <c r="N1" t="s">
+        <v>178</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q1" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="G1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" t="s">
-        <v>171</v>
-      </c>
-      <c r="K1" t="s">
-        <v>172</v>
-      </c>
-      <c r="M1" t="s">
-        <v>176</v>
-      </c>
-      <c r="N1" t="s">
-        <v>177</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>211</v>
-      </c>
       <c r="S1" s="4" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="W1" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="X1" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y1" t="s">
         <v>245</v>
-      </c>
-      <c r="X1" t="s">
-        <v>243</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="V2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>316</v>
+        <v>274</v>
       </c>
       <c r="C3" t="s">
-        <v>314</v>
+        <v>276</v>
       </c>
       <c r="E3" s="4" t="str">
         <f>C3</f>
-        <v>Log</v>
+        <v>Template</v>
       </c>
       <c r="G3" s="3" t="str">
         <f>LOWER(B3)</f>
-        <v>logreceiver</v>
+        <v>templatemanagement</v>
       </c>
       <c r="H3" s="3" t="str">
         <f>Application!$D$5&amp;"."&amp;G3</f>
-        <v>org.xlbean.logreceiver</v>
+        <v>com.templengine.templatemanagement</v>
       </c>
       <c r="J3" s="3" t="str">
         <f>H3&amp;".entity"</f>
-        <v>org.xlbean.logreceiver.entity</v>
+        <v>com.templengine.templatemanagement.entity</v>
       </c>
       <c r="K3" s="3" t="str">
         <f>C3</f>
-        <v>Log</v>
+        <v>Template</v>
       </c>
       <c r="M3" s="3" t="str">
         <f>H3&amp;".dao"</f>
-        <v>org.xlbean.logreceiver.dao</v>
+        <v>com.templengine.templatemanagement.dao</v>
       </c>
       <c r="N3" s="3" t="str">
         <f>C3&amp;"Dao"</f>
-        <v>LogDao</v>
+        <v>TemplateDao</v>
       </c>
       <c r="P3" s="3" t="str">
         <f>M3&amp;".mapper"</f>
-        <v>org.xlbean.logreceiver.dao.mapper</v>
+        <v>com.templengine.templatemanagement.dao.mapper</v>
       </c>
       <c r="Q3" s="3" t="str">
         <f>K3&amp;"Mapper"</f>
-        <v>LogMapper</v>
+        <v>TemplateMapper</v>
       </c>
       <c r="S3" s="3" t="str">
         <f>M3&amp;".mapper.gen"</f>
-        <v>org.xlbean.logreceiver.dao.mapper.gen</v>
+        <v>com.templengine.templatemanagement.dao.mapper.gen</v>
       </c>
       <c r="T3" s="3" t="str">
         <f>K3&amp;"MapperGen"</f>
-        <v>LogMapperGen</v>
+        <v>TemplateMapperGen</v>
       </c>
       <c r="V3" t="s">
-        <v>317</v>
+        <v>279</v>
       </c>
       <c r="W3" s="7" t="str">
         <f>"/"&amp;LOWER(B3)&amp;V3</f>
-        <v>/logreceiver/logs</v>
+        <v>/templatemanagement/templates</v>
       </c>
       <c r="X3" s="3" t="str">
         <f>H3&amp;".api"</f>
-        <v>org.xlbean.logreceiver.api</v>
+        <v>com.templengine.templatemanagement.api</v>
       </c>
       <c r="Y3" s="3" t="str">
         <f>C3&amp;"Api"</f>
-        <v>LogApi</v>
+        <v>TemplateApi</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="9"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
+      <c r="B4" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E4" s="4" t="str">
+        <f t="shared" ref="E4" si="0">C4</f>
+        <v>TemplateParameter</v>
+      </c>
+      <c r="G4" s="3" t="str">
+        <f t="shared" ref="G4" si="1">LOWER(B4)</f>
+        <v>templatemanagement</v>
+      </c>
+      <c r="H4" s="3" t="str">
+        <f>Application!$D$5&amp;"."&amp;G4</f>
+        <v>com.templengine.templatemanagement</v>
+      </c>
+      <c r="J4" s="3" t="str">
+        <f t="shared" ref="J4" si="2">H4&amp;".entity"</f>
+        <v>com.templengine.templatemanagement.entity</v>
+      </c>
+      <c r="K4" s="3" t="str">
+        <f t="shared" ref="K4" si="3">C4</f>
+        <v>TemplateParameter</v>
+      </c>
+      <c r="M4" s="3" t="str">
+        <f t="shared" ref="M4" si="4">H4&amp;".dao"</f>
+        <v>com.templengine.templatemanagement.dao</v>
+      </c>
+      <c r="N4" s="3" t="str">
+        <f t="shared" ref="N4" si="5">C4&amp;"Dao"</f>
+        <v>TemplateParameterDao</v>
+      </c>
+      <c r="P4" s="3" t="str">
+        <f t="shared" ref="P4" si="6">M4&amp;".mapper"</f>
+        <v>com.templengine.templatemanagement.dao.mapper</v>
+      </c>
+      <c r="Q4" s="3" t="str">
+        <f t="shared" ref="Q4" si="7">K4&amp;"Mapper"</f>
+        <v>TemplateParameterMapper</v>
+      </c>
+      <c r="S4" s="3" t="str">
+        <f t="shared" ref="S4" si="8">M4&amp;".mapper.gen"</f>
+        <v>com.templengine.templatemanagement.dao.mapper.gen</v>
+      </c>
+      <c r="T4" s="3" t="str">
+        <f t="shared" ref="T4" si="9">K4&amp;"MapperGen"</f>
+        <v>TemplateParameterMapperGen</v>
+      </c>
+      <c r="V4" t="s">
+        <v>280</v>
+      </c>
+      <c r="W4" s="7" t="str">
+        <f t="shared" ref="W4" si="10">"/"&amp;LOWER(B4)&amp;V4</f>
+        <v>/templatemanagement/templates/{templateId}/parameters</v>
+      </c>
+      <c r="X4" s="3" t="str">
+        <f t="shared" ref="X4" si="11">H4&amp;".api"</f>
+        <v>com.templengine.templatemanagement.api</v>
+      </c>
+      <c r="Y4" s="3" t="str">
+        <f t="shared" ref="Y4" si="12">C4&amp;"Api"</f>
+        <v>TemplateParameterApi</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="9"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="J5" s="3"/>
@@ -3756,6 +3858,20 @@
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
     </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3765,10 +3881,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD9"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -3792,90 +3908,90 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
         <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="M1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="N1" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="O1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="P1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="Q1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="R1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="S1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="T1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="U1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="V1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="W1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="Y1" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>268</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC1" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="Z1" t="s">
-        <v>267</v>
-      </c>
-      <c r="AA1" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>270</v>
-      </c>
       <c r="AD1" s="8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
         <v>83</v>
@@ -3893,64 +4009,64 @@
         <v>119</v>
       </c>
       <c r="H2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K2" t="s">
+        <v>249</v>
+      </c>
+      <c r="L2" t="s">
         <v>248</v>
       </c>
-      <c r="L2" t="s">
-        <v>247</v>
-      </c>
       <c r="M2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="N2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="P2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="Q2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="R2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="V2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Z2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AA2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AB2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AD2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B3" s="3" t="str">
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C3,Entities!$C$3:$C$5,0))</f>
+        <v>TemplateManagement</v>
+      </c>
+      <c r="C3" t="s">
         <v>275</v>
       </c>
-      <c r="B3" s="3" t="str">
-        <f>INDEX(Entities!$B$3:$B$4,MATCH(EntityProperties!C3,Entities!$C$3:$C$4,0))</f>
-        <v>LogReceiver</v>
-      </c>
-      <c r="C3" t="s">
-        <v>318</v>
-      </c>
       <c r="D3" t="s">
-        <v>319</v>
+        <v>282</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3963,15 +4079,15 @@
       </c>
       <c r="K3" s="3" t="str">
         <f>UPPER(B3)</f>
-        <v>LOGRECEIVER</v>
+        <v>TEMPLATEMANAGEMENT</v>
       </c>
       <c r="L3" s="3" t="str">
         <f>VLOOKUP(C3,Entities!C:E,3,FALSE)</f>
-        <v>Log</v>
+        <v>Template</v>
       </c>
       <c r="M3" s="3" t="str">
         <f>D3</f>
-        <v>logId</v>
+        <v>templateId</v>
       </c>
       <c r="N3" s="3">
         <f>IF(L3=L2,N2+1,1)</f>
@@ -4004,39 +4120,39 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3" t="str">
-        <f>INDEX(Entities!$B$3:$B$4,MATCH(EntityProperties!C4,Entities!$C$3:$C$4,0))</f>
-        <v>LogReceiver</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>318</v>
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C4,Entities!$C$3:$C$5,0))</f>
+        <v>TemplateManagement</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>275</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F4" t="s">
         <v>123</v>
       </c>
       <c r="G4">
-        <v>1000000</v>
+        <v>128</v>
       </c>
       <c r="K4" s="3" t="str">
         <f t="shared" ref="K4" si="0">UPPER(B4)</f>
-        <v>LOGRECEIVER</v>
+        <v>TEMPLATEMANAGEMENT</v>
       </c>
       <c r="L4" s="3" t="str">
         <f>VLOOKUP(C4,Entities!C:E,3,FALSE)</f>
-        <v>Log</v>
+        <v>Template</v>
       </c>
       <c r="M4" s="3" t="str">
         <f t="shared" ref="M4" si="1">D4</f>
-        <v>data</v>
+        <v>name</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" ref="N4" si="2">IF(L4=L3,N3+1,1)</f>
         <v>2</v>
       </c>
       <c r="P4" s="6" t="str">
-        <f t="shared" ref="P4" si="3">IF(E4=1,"NO","YES")</f>
+        <f t="shared" ref="P4:P12" si="3">IF(E4=1,"NO","YES")</f>
         <v>YES</v>
       </c>
       <c r="Q4" s="3" t="str">
@@ -4044,114 +4160,585 @@
         <v>varchar</v>
       </c>
       <c r="R4" s="3">
-        <f t="shared" ref="R4" si="4">IF(OR(Q4="char",Q4="varchar"),IF(G4="-",50,G4),IF(Q4="int",11,""))</f>
+        <f t="shared" ref="R4:R12" si="4">IF(OR(Q4="char",Q4="varchar"),IF(G4="-",50,G4),IF(Q4="int",11,""))</f>
+        <v>128</v>
+      </c>
+      <c r="V4" s="3" t="str">
+        <f t="shared" ref="V4:V12" si="5">IF(R4="",Q4,Q4&amp;"("&amp;R4&amp;")")</f>
+        <v>varchar(128)</v>
+      </c>
+      <c r="Y4" s="8" t="str">
+        <f t="shared" ref="Y4:Y17" si="6">IF(E4&lt;&gt;"","NotNull","")</f>
+        <v/>
+      </c>
+      <c r="AC4">
+        <f t="shared" ref="AC4:AC17" si="7">IF(G4&lt;&gt;"-",G4,"")</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="3" t="str">
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C5,Entities!$C$3:$C$5,0))</f>
+        <v>TemplateManagement</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1024</v>
+      </c>
+      <c r="K5" s="3" t="str">
+        <f t="shared" ref="K5:K6" si="8">UPPER(B5)</f>
+        <v>TEMPLATEMANAGEMENT</v>
+      </c>
+      <c r="L5" s="3" t="str">
+        <f>VLOOKUP(C5,Entities!C:E,3,FALSE)</f>
+        <v>Template</v>
+      </c>
+      <c r="M5" s="3" t="str">
+        <f t="shared" ref="M5:M6" si="9">D5</f>
+        <v>description</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" ref="N5:N6" si="10">IF(L5=L4,N4+1,1)</f>
+        <v>3</v>
+      </c>
+      <c r="P5" s="11" t="str">
+        <f t="shared" ref="P5:P6" si="11">IF(E5=1,"NO","YES")</f>
+        <v>YES</v>
+      </c>
+      <c r="Q5" s="3" t="str">
+        <f>VLOOKUP(F5,vlookup!$B:$C,2,FALSE)</f>
+        <v>varchar</v>
+      </c>
+      <c r="R5" s="3">
+        <f t="shared" ref="R5:R6" si="12">IF(OR(Q5="char",Q5="varchar"),IF(G5="-",50,G5),IF(Q5="int",11,""))</f>
+        <v>1024</v>
+      </c>
+      <c r="V5" s="3" t="str">
+        <f t="shared" ref="V5:V6" si="13">IF(R5="",Q5,Q5&amp;"("&amp;R5&amp;")")</f>
+        <v>varchar(1024)</v>
+      </c>
+      <c r="Y5" s="11" t="str">
+        <f t="shared" ref="Y5:Y6" si="14">IF(E5&lt;&gt;"","NotNull","")</f>
+        <v/>
+      </c>
+      <c r="AC5" s="11">
+        <f t="shared" ref="AC5:AC6" si="15">IF(G5&lt;&gt;"-",G5,"")</f>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="3" t="str">
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C6,Entities!$C$3:$C$5,0))</f>
+        <v>TemplateManagement</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="G6" s="11">
+        <v>512</v>
+      </c>
+      <c r="K6" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>TEMPLATEMANAGEMENT</v>
+      </c>
+      <c r="L6" s="3" t="str">
+        <f>VLOOKUP(C6,Entities!C:E,3,FALSE)</f>
+        <v>Template</v>
+      </c>
+      <c r="M6" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>path</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="P6" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>YES</v>
+      </c>
+      <c r="Q6" s="3" t="str">
+        <f>VLOOKUP(F6,vlookup!$B:$C,2,FALSE)</f>
+        <v>varchar</v>
+      </c>
+      <c r="R6" s="3">
+        <f t="shared" si="12"/>
+        <v>512</v>
+      </c>
+      <c r="V6" s="3" t="str">
+        <f t="shared" si="13"/>
+        <v>varchar(512)</v>
+      </c>
+      <c r="Y6" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="AC6" s="11">
+        <f t="shared" si="15"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="3" t="str">
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C7,Entities!$C$3:$C$5,0))</f>
+        <v>TemplateManagement</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="G7" s="11">
         <v>1000000</v>
       </c>
-      <c r="V4" s="3" t="str">
-        <f t="shared" ref="V4" si="5">IF(R4="",Q4,Q4&amp;"("&amp;R4&amp;")")</f>
+      <c r="K7" s="3" t="str">
+        <f t="shared" ref="K7" si="16">UPPER(B7)</f>
+        <v>TEMPLATEMANAGEMENT</v>
+      </c>
+      <c r="L7" s="3" t="str">
+        <f>VLOOKUP(C7,Entities!C:E,3,FALSE)</f>
+        <v>Template</v>
+      </c>
+      <c r="M7" s="3" t="str">
+        <f t="shared" ref="M7" si="17">D7</f>
+        <v>content</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" ref="N7:N12" si="18">IF(L7=L6,N6+1,1)</f>
+        <v>5</v>
+      </c>
+      <c r="P7" s="11" t="str">
+        <f t="shared" ref="P7" si="19">IF(E7=1,"NO","YES")</f>
+        <v>YES</v>
+      </c>
+      <c r="Q7" s="3" t="str">
+        <f>VLOOKUP(F7,vlookup!$B:$C,2,FALSE)</f>
+        <v>varchar</v>
+      </c>
+      <c r="R7" s="3">
+        <f t="shared" ref="R7" si="20">IF(OR(Q7="char",Q7="varchar"),IF(G7="-",50,G7),IF(Q7="int",11,""))</f>
+        <v>1000000</v>
+      </c>
+      <c r="V7" s="3" t="str">
+        <f t="shared" ref="V7" si="21">IF(R7="",Q7,Q7&amp;"("&amp;R7&amp;")")</f>
         <v>varchar(1000000)</v>
       </c>
-      <c r="Y4" s="8" t="str">
-        <f t="shared" ref="Y4:Y9" si="6">IF(E4&lt;&gt;"","NotNull","")</f>
+      <c r="Y7" s="11" t="str">
+        <f t="shared" ref="Y7" si="22">IF(E7&lt;&gt;"","NotNull","")</f>
         <v/>
       </c>
-      <c r="AC4">
-        <f t="shared" ref="AC4:AC9" si="7">IF(G4&lt;&gt;"-",G4,"")</f>
+      <c r="AC7" s="11">
+        <f t="shared" ref="AC7" si="23">IF(G7&lt;&gt;"-",G7,"")</f>
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="3"/>
-      <c r="C5" s="9"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="V5" s="3"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="3"/>
-      <c r="C6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="V6" s="3"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="Y7" s="8" t="str">
+    <row r="8" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="3" t="str">
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C8,Entities!$C$3:$C$5,0))</f>
+        <v>TemplateManagement</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="G8" s="11">
+        <v>20</v>
+      </c>
+      <c r="K8" s="3" t="str">
+        <f t="shared" ref="K8" si="24">UPPER(B8)</f>
+        <v>TEMPLATEMANAGEMENT</v>
+      </c>
+      <c r="L8" s="3" t="str">
+        <f>VLOOKUP(C8,Entities!C:E,3,FALSE)</f>
+        <v>Template</v>
+      </c>
+      <c r="M8" s="3" t="str">
+        <f t="shared" ref="M8" si="25">D8</f>
+        <v>contentType</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" ref="N8" si="26">IF(L8=L7,N7+1,1)</f>
+        <v>6</v>
+      </c>
+      <c r="P8" s="11" t="str">
+        <f t="shared" ref="P8" si="27">IF(E8=1,"NO","YES")</f>
+        <v>YES</v>
+      </c>
+      <c r="Q8" s="3" t="str">
+        <f>VLOOKUP(F8,vlookup!$B:$C,2,FALSE)</f>
+        <v>varchar</v>
+      </c>
+      <c r="R8" s="3">
+        <f t="shared" ref="R8" si="28">IF(OR(Q8="char",Q8="varchar"),IF(G8="-",50,G8),IF(Q8="int",11,""))</f>
+        <v>20</v>
+      </c>
+      <c r="V8" s="3" t="str">
+        <f t="shared" ref="V8" si="29">IF(R8="",Q8,Q8&amp;"("&amp;R8&amp;")")</f>
+        <v>varchar(20)</v>
+      </c>
+      <c r="Y8" s="11" t="str">
+        <f t="shared" ref="Y8" si="30">IF(E8&lt;&gt;"","NotNull","")</f>
+        <v/>
+      </c>
+      <c r="AC8" s="11">
+        <f t="shared" ref="AC8" si="31">IF(G8&lt;&gt;"-",G8,"")</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="3" t="str">
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C9,Entities!$C$3:$C$5,0))</f>
+        <v>TemplateManagement</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="G9" s="11">
+        <v>10000</v>
+      </c>
+      <c r="K9" s="3" t="str">
+        <f t="shared" ref="K9" si="32">UPPER(B9)</f>
+        <v>TEMPLATEMANAGEMENT</v>
+      </c>
+      <c r="L9" s="3" t="str">
+        <f>VLOOKUP(C9,Entities!C:E,3,FALSE)</f>
+        <v>Template</v>
+      </c>
+      <c r="M9" s="3" t="str">
+        <f t="shared" ref="M9" si="33">D9</f>
+        <v>sampleDataJsonStr</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" ref="N9" si="34">IF(L9=L7,N7+1,1)</f>
+        <v>6</v>
+      </c>
+      <c r="P9" s="11" t="str">
+        <f t="shared" ref="P9" si="35">IF(E9=1,"NO","YES")</f>
+        <v>YES</v>
+      </c>
+      <c r="Q9" s="3" t="str">
+        <f>VLOOKUP(F9,vlookup!$B:$C,2,FALSE)</f>
+        <v>varchar</v>
+      </c>
+      <c r="R9" s="3">
+        <f t="shared" ref="R9" si="36">IF(OR(Q9="char",Q9="varchar"),IF(G9="-",50,G9),IF(Q9="int",11,""))</f>
+        <v>10000</v>
+      </c>
+      <c r="V9" s="3" t="str">
+        <f t="shared" ref="V9" si="37">IF(R9="",Q9,Q9&amp;"("&amp;R9&amp;")")</f>
+        <v>varchar(10000)</v>
+      </c>
+      <c r="Y9" s="11" t="str">
+        <f t="shared" ref="Y9" si="38">IF(E9&lt;&gt;"","NotNull","")</f>
+        <v/>
+      </c>
+      <c r="AC9" s="11">
+        <f t="shared" ref="AC9" si="39">IF(G9&lt;&gt;"-",G9,"")</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="3" t="str">
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C10,Entities!$C$3:$C$5,0))</f>
+        <v>TemplateManagement</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D10" t="s">
+        <v>281</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="3" t="str">
+        <f t="shared" ref="K10:K12" si="40">UPPER(B10)</f>
+        <v>TEMPLATEMANAGEMENT</v>
+      </c>
+      <c r="L10" s="3" t="str">
+        <f>VLOOKUP(C10,Entities!C:E,3,FALSE)</f>
+        <v>TemplateParameter</v>
+      </c>
+      <c r="M10" s="3" t="str">
+        <f t="shared" ref="M10:M12" si="41">D10</f>
+        <v>templateId</v>
+      </c>
+      <c r="N10" s="3">
+        <f>IF(L10=L7,N7+1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="P10" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>NO</v>
+      </c>
+      <c r="Q10" s="3" t="str">
+        <f>VLOOKUP(F10,vlookup!$B:$C,2,FALSE)</f>
+        <v>int</v>
+      </c>
+      <c r="R10" s="3">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="V10" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>int(11)</v>
+      </c>
+      <c r="Y10" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>NotNull</v>
+      </c>
+      <c r="AC10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="3" t="str">
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C11,Entities!$C$3:$C$5,0))</f>
+        <v>TemplateManagement</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" t="s">
+        <v>128</v>
+      </c>
+      <c r="K11" s="3" t="str">
+        <f t="shared" si="40"/>
+        <v>TEMPLATEMANAGEMENT</v>
+      </c>
+      <c r="L11" s="3" t="str">
+        <f>VLOOKUP(C11,Entities!C:E,3,FALSE)</f>
+        <v>TemplateParameter</v>
+      </c>
+      <c r="M11" s="3" t="str">
+        <f t="shared" si="41"/>
+        <v>parameterId</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="P11" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>YES</v>
+      </c>
+      <c r="Q11" s="3" t="str">
+        <f>VLOOKUP(F11,vlookup!$B:$C,2,FALSE)</f>
+        <v>int</v>
+      </c>
+      <c r="R11" s="3">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="V11" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>int(11)</v>
+      </c>
+      <c r="Y11" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>NotNull</v>
+      </c>
+      <c r="AC11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="3" t="str">
+        <f>INDEX(Entities!$B$3:$B$5,MATCH(EntityProperties!C12,Entities!$C$3:$C$5,0))</f>
+        <v>TemplateManagement</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D12" t="s">
+        <v>284</v>
+      </c>
+      <c r="F12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12">
+        <v>255</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="K12" s="3" t="str">
+        <f t="shared" si="40"/>
+        <v>TEMPLATEMANAGEMENT</v>
+      </c>
+      <c r="L12" s="3" t="str">
+        <f>VLOOKUP(C12,Entities!C:E,3,FALSE)</f>
+        <v>TemplateParameter</v>
+      </c>
+      <c r="M12" s="3" t="str">
+        <f t="shared" si="41"/>
+        <v>parameterName</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="P12" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>YES</v>
+      </c>
+      <c r="Q12" s="3" t="str">
+        <f>VLOOKUP(F12,vlookup!$B:$C,2,FALSE)</f>
+        <v>varchar</v>
+      </c>
+      <c r="R12" s="3">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="V12" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>varchar(255)</v>
+      </c>
+      <c r="Y12" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AC7">
+      <c r="AC12">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="3"/>
+      <c r="C13" s="9"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="V13" s="3"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="3"/>
+      <c r="C14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="V14" s="3"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="Y15" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AC15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="Y8" s="8" t="str">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="Y16" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AC8">
+      <c r="AC16">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="Y9" s="8" t="str">
+    <row r="17" spans="2:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="Y17" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AC9">
+      <c r="AC17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD6" xr:uid="{B02FBA99-861D-4255-8BEE-D719BA83889D}"/>
+  <autoFilter ref="A1:AD14" xr:uid="{B02FBA99-861D-4255-8BEE-D719BA83889D}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="Z3:AA9">
+  <conditionalFormatting sqref="Z3:AA17">
     <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND($F3&lt;&gt;"Integer")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AD9">
+  <conditionalFormatting sqref="AB3:AD17">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>NOT($F3="String")</formula>
     </cfRule>
@@ -4165,13 +4752,13 @@
           <x14:formula1>
             <xm:f>List!$B$2:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>Y3:Y9</xm:sqref>
+          <xm:sqref>Y3:Y17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B0F9129-3A24-4315-8826-417A47D2DED6}">
           <x14:formula1>
             <xm:f>vlookup!$B$2:$B$20</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F9</xm:sqref>
+          <xm:sqref>F3:F17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4212,78 +4799,78 @@
         <v>0</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="N1" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="Y1" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="O1" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="W1" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>292</v>
-      </c>
       <c r="Z1" s="10" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="AA1" s="10" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
       <c r="AB1" s="10" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="AC1" s="10" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="AD1" s="10" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>83</v>
@@ -4301,10 +4888,10 @@
         <v>119</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>53</v>
@@ -4313,7 +4900,7 @@
         <v>54</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="P2" s="10" t="s">
         <v>58</v>
@@ -4328,35 +4915,35 @@
         <v>65</v>
       </c>
       <c r="Y2" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Z2" s="10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AA2" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AB2" s="10" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AC2" s="10" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AD2" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="10" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="10" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>72</v>
@@ -4402,7 +4989,7 @@
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="10" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>123</v>
@@ -4452,10 +5039,10 @@
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="10" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>72</v>
@@ -4502,7 +5089,7 @@
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="10" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>123</v>
@@ -4668,74 +5255,74 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" t="s">
         <v>203</v>
       </c>
-      <c r="B1" t="s">
-        <v>202</v>
-      </c>
       <c r="C1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4766,92 +5353,92 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>218</v>
-      </c>
       <c r="H1" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="G2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" t="s">
+        <v>237</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="L2" t="s">
         <v>232</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="G2" t="s">
-        <v>213</v>
-      </c>
-      <c r="H2" t="s">
-        <v>236</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="L2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H3" t="s">
         <v>95</v>
       </c>
       <c r="L3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -4859,16 +5446,16 @@
         <v>82</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G4" t="s">
         <v>112</v>
       </c>
       <c r="H4" t="s">
+        <v>231</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -4894,15 +5481,15 @@
   <sheetData>
     <row r="1" spans="2:3" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
@@ -4910,15 +5497,15 @@
         <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
@@ -4926,7 +5513,7 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
@@ -4934,7 +5521,7 @@
         <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.55000000000000004">
@@ -4942,15 +5529,15 @@
         <v>122</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="C8" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -4975,25 +5562,25 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>